<commit_message>
release symlex overall exe file tested
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_44.xlsx
+++ b/test_case_report/sprint_44.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB47AB20-BBB6-401A-984B-07E68E7366C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8188038B-C593-4173-8927-CD8A24286C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,34 +31,34 @@
     <t>Total Review</t>
   </si>
   <si>
-    <t>Spint( 43) - Day 1 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 2 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 3 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 4 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 5 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 6 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 7 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 8 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 9 - Test Case Summary</t>
-  </si>
-  <si>
-    <t>Spint( 43) - Day 10 - Test Case Summary</t>
+    <t>Spint( 44) - Day 1 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 2 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 3 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 4 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 5 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 6 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 7 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 8 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 9 - Test Case Summary</t>
+  </si>
+  <si>
+    <t>Spint( 44) - Day 10 - Test Case Summary</t>
   </si>
 </sst>
 </file>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -584,19 +584,25 @@
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>7075</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="18">
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>2610</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="18">
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5">
+        <v>2610</v>
+      </c>
     </row>
     <row r="14" spans="2:3" ht="18.75" customHeight="1">
       <c r="B14" s="6" t="s">
@@ -608,19 +614,25 @@
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>7075</v>
+      </c>
     </row>
     <row r="16" spans="2:3" ht="18">
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>2610</v>
+      </c>
     </row>
     <row r="17" spans="2:3" ht="18">
       <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>2610</v>
+      </c>
     </row>
     <row r="20" spans="2:3" ht="18">
       <c r="B20" s="6" t="s">
@@ -632,19 +644,25 @@
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>7075</v>
+      </c>
     </row>
     <row r="22" spans="2:3" ht="18">
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4">
+        <v>2660</v>
+      </c>
     </row>
     <row r="23" spans="2:3" ht="18">
       <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>2660</v>
+      </c>
     </row>
     <row r="26" spans="2:3" ht="18">
       <c r="B26" s="6" t="s">

</xml_diff>

<commit_message>
windows check for new release and ui test case written
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_44.xlsx
+++ b/test_case_report/sprint_44.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0C1CB9-7B53-4115-A071-EED5289C8821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E627499-0427-4EE7-9306-020BD645CACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -734,19 +734,25 @@
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2">
+        <v>7075</v>
+      </c>
     </row>
     <row r="40" spans="2:3" ht="18">
       <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="4"/>
+      <c r="C40" s="4">
+        <v>2790</v>
+      </c>
     </row>
     <row r="41" spans="2:3" ht="18">
       <c r="B41" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="5"/>
+      <c r="C41" s="5">
+        <v>2790</v>
+      </c>
     </row>
     <row r="44" spans="2:3" ht="18">
       <c r="B44" s="6" t="s">
@@ -758,19 +764,25 @@
       <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2">
+        <v>7103</v>
+      </c>
     </row>
     <row r="46" spans="2:3" ht="18">
       <c r="B46" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="4">
+        <v>2850</v>
+      </c>
     </row>
     <row r="47" spans="2:3" ht="18">
       <c r="B47" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="5"/>
+      <c r="C47" s="5">
+        <v>2850</v>
+      </c>
     </row>
     <row r="50" spans="2:3" ht="18">
       <c r="B50" s="6" t="s">
@@ -782,19 +794,25 @@
       <c r="B51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2">
+        <v>7131</v>
+      </c>
     </row>
     <row r="52" spans="2:3" ht="18">
       <c r="B52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="4">
+        <v>2880</v>
+      </c>
     </row>
     <row r="53" spans="2:3" ht="18">
       <c r="B53" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="5">
+        <v>2880</v>
+      </c>
     </row>
     <row r="57" spans="2:3" ht="18">
       <c r="B57" s="6" t="s">

</xml_diff>